<commit_message>
RL agent has now sink speed
</commit_message>
<xml_diff>
--- a/pyFiles/RL/Results/New Results/ResultsDQNfixEpsilon.xlsx
+++ b/pyFiles/RL/Results/New Results/ResultsDQNfixEpsilon.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bozho1\Desktop\Thesis Code\ThesisWorkCybercom\pyFiles\RL\Results\New Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01E9FE89-F97D-4BCC-B949-8E155632ECFB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{729A3D91-2F0E-48EF-9BBC-3C4B1985314F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{1BC5E51A-5632-4252-887C-9C128D35FB87}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1BC5E51A-5632-4252-887C-9C128D35FB87}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="31">
   <si>
     <t>Controller</t>
   </si>
@@ -144,6 +144,9 @@
   </si>
   <si>
     <t>Until All Node Dies</t>
+  </si>
+  <si>
+    <t>Sink Speed Tests</t>
   </si>
 </sst>
 </file>
@@ -591,10 +594,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2693EA75-5C63-4FDE-887F-C7326CFE699C}">
-  <dimension ref="A1:AN159"/>
+  <dimension ref="A1:AN213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="Z165" sqref="Z165"/>
+    <sheetView tabSelected="1" topLeftCell="A128" workbookViewId="0">
+      <selection activeCell="H216" sqref="H216"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8055,7 +8058,7 @@
         <v>2.2352497999999899</v>
       </c>
       <c r="Z123">
-        <f t="shared" ref="Z123:Z159" si="14">W123/Y123</f>
+        <f t="shared" ref="Z123:Z156" si="14">W123/Y123</f>
         <v>4922.044954438672</v>
       </c>
       <c r="AB123">
@@ -8077,7 +8080,7 @@
         <v>4.9999999999999902</v>
       </c>
       <c r="AK123">
-        <f t="shared" ref="AK123:AK158" si="15">AH123/AJ123</f>
+        <f t="shared" ref="AK123:AK156" si="15">AH123/AJ123</f>
         <v>5847.6000000000113</v>
       </c>
       <c r="AM123">
@@ -10267,6 +10270,947 @@
       <c r="AK159">
         <f>AH159/AJ159</f>
         <v>6433.7800000000125</v>
+      </c>
+    </row>
+    <row r="160" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A160" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="161" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A161" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="L161" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="162" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A162" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="L162" s="10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="163" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A163" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B163" t="s">
+        <v>12</v>
+      </c>
+      <c r="L163" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="M163" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="164" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A164" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B164" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C164" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D164" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="G164" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="H164" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="L164" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="M164" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="N164" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="O164" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="R164" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="S164" s="13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="165" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A165" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G165">
+        <v>1</v>
+      </c>
+      <c r="H165" t="s">
+        <v>8</v>
+      </c>
+      <c r="L165" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="R165">
+        <v>1</v>
+      </c>
+      <c r="S165" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="166" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A166" s="1">
+        <v>1</v>
+      </c>
+      <c r="G166">
+        <v>1</v>
+      </c>
+      <c r="H166" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L166" s="1">
+        <v>1</v>
+      </c>
+      <c r="R166">
+        <v>1</v>
+      </c>
+      <c r="S166" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="167" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A167" s="1">
+        <v>2</v>
+      </c>
+      <c r="G167">
+        <v>1</v>
+      </c>
+      <c r="H167" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L167" s="1">
+        <v>2</v>
+      </c>
+      <c r="R167">
+        <v>1</v>
+      </c>
+      <c r="S167" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="168" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A168" s="1">
+        <v>3</v>
+      </c>
+      <c r="G168">
+        <v>1</v>
+      </c>
+      <c r="H168" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L168" s="1">
+        <v>3</v>
+      </c>
+      <c r="R168">
+        <v>1</v>
+      </c>
+      <c r="S168" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="169" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A169" s="1">
+        <v>4</v>
+      </c>
+      <c r="G169">
+        <v>1</v>
+      </c>
+      <c r="H169" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L169" s="1">
+        <v>4</v>
+      </c>
+      <c r="R169">
+        <v>1</v>
+      </c>
+      <c r="S169" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="170" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A170" s="1">
+        <v>5</v>
+      </c>
+      <c r="G170">
+        <v>1</v>
+      </c>
+      <c r="H170" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L170" s="1">
+        <v>5</v>
+      </c>
+      <c r="R170">
+        <v>1</v>
+      </c>
+      <c r="S170" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="171" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A171" s="1">
+        <v>6</v>
+      </c>
+      <c r="G171">
+        <v>1</v>
+      </c>
+      <c r="H171" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L171" s="1">
+        <v>6</v>
+      </c>
+      <c r="R171">
+        <v>1</v>
+      </c>
+      <c r="S171" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="172" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A172" s="1">
+        <v>7</v>
+      </c>
+      <c r="G172">
+        <v>1</v>
+      </c>
+      <c r="H172" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L172" s="1">
+        <v>7</v>
+      </c>
+      <c r="R172">
+        <v>1</v>
+      </c>
+      <c r="S172" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="173" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A173" s="1">
+        <v>8</v>
+      </c>
+      <c r="G173">
+        <v>1</v>
+      </c>
+      <c r="H173" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L173" s="1">
+        <v>8</v>
+      </c>
+      <c r="R173">
+        <v>1</v>
+      </c>
+      <c r="S173" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="174" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A174" s="4">
+        <v>9</v>
+      </c>
+      <c r="G174">
+        <v>1</v>
+      </c>
+      <c r="H174" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L174" s="4">
+        <v>9</v>
+      </c>
+      <c r="R174">
+        <v>1</v>
+      </c>
+      <c r="S174" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="175" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A175" s="1">
+        <v>10</v>
+      </c>
+      <c r="G175">
+        <v>1</v>
+      </c>
+      <c r="H175" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L175" s="1">
+        <v>10</v>
+      </c>
+      <c r="R175">
+        <v>1</v>
+      </c>
+      <c r="S175" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="176" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A176" s="1">
+        <v>11</v>
+      </c>
+      <c r="G176">
+        <v>0.05</v>
+      </c>
+      <c r="H176" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L176" s="1">
+        <v>11</v>
+      </c>
+      <c r="R176">
+        <v>0.05</v>
+      </c>
+      <c r="S176" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="177" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A177" s="1">
+        <v>12</v>
+      </c>
+      <c r="G177">
+        <v>0.05</v>
+      </c>
+      <c r="H177" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L177" s="1">
+        <v>12</v>
+      </c>
+      <c r="R177">
+        <v>0.05</v>
+      </c>
+      <c r="S177" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="178" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A178" s="1">
+        <v>13</v>
+      </c>
+      <c r="G178">
+        <v>0.05</v>
+      </c>
+      <c r="H178" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L178" s="1">
+        <v>13</v>
+      </c>
+      <c r="R178">
+        <v>0.05</v>
+      </c>
+      <c r="S178" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="179" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A179" s="1">
+        <v>14</v>
+      </c>
+      <c r="G179">
+        <v>0.05</v>
+      </c>
+      <c r="H179" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L179" s="1">
+        <v>14</v>
+      </c>
+      <c r="R179">
+        <v>0.05</v>
+      </c>
+      <c r="S179" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="180" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A180" s="1">
+        <v>15</v>
+      </c>
+      <c r="G180">
+        <v>0.05</v>
+      </c>
+      <c r="H180" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L180" s="1">
+        <v>15</v>
+      </c>
+      <c r="R180">
+        <v>0.05</v>
+      </c>
+      <c r="S180" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="181" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A181" s="1">
+        <v>16</v>
+      </c>
+      <c r="G181">
+        <v>0.05</v>
+      </c>
+      <c r="H181" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L181" s="1">
+        <v>16</v>
+      </c>
+      <c r="R181">
+        <v>0.05</v>
+      </c>
+      <c r="S181" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="182" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A182" s="1">
+        <v>17</v>
+      </c>
+      <c r="G182">
+        <v>0.05</v>
+      </c>
+      <c r="H182" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L182" s="1">
+        <v>17</v>
+      </c>
+      <c r="R182">
+        <v>0.05</v>
+      </c>
+      <c r="S182" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="183" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A183" s="1">
+        <v>18</v>
+      </c>
+      <c r="G183">
+        <v>0.05</v>
+      </c>
+      <c r="H183" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L183" s="1">
+        <v>18</v>
+      </c>
+      <c r="R183">
+        <v>0.05</v>
+      </c>
+      <c r="S183" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="184" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A184" s="1">
+        <v>19</v>
+      </c>
+      <c r="G184">
+        <v>0.05</v>
+      </c>
+      <c r="H184" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L184" s="1">
+        <v>19</v>
+      </c>
+      <c r="R184">
+        <v>0.05</v>
+      </c>
+      <c r="S184" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="185" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A185" s="1">
+        <v>20</v>
+      </c>
+      <c r="G185">
+        <v>0.05</v>
+      </c>
+      <c r="H185" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L185" s="1">
+        <v>20</v>
+      </c>
+      <c r="R185">
+        <v>0.05</v>
+      </c>
+      <c r="S185" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="186" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A186" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="L186" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="187" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A187" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="L187" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="188" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B188" s="6"/>
+    </row>
+    <row r="190" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A190" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="L190" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="191" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A191" s="1">
+        <v>1</v>
+      </c>
+      <c r="G191">
+        <v>1</v>
+      </c>
+      <c r="H191" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L191" s="1">
+        <v>1</v>
+      </c>
+      <c r="R191">
+        <v>1</v>
+      </c>
+      <c r="S191" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="192" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A192" s="1">
+        <v>2</v>
+      </c>
+      <c r="G192">
+        <v>1</v>
+      </c>
+      <c r="H192" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L192" s="1">
+        <v>2</v>
+      </c>
+      <c r="R192">
+        <v>1</v>
+      </c>
+      <c r="S192" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="193" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A193" s="1">
+        <v>3</v>
+      </c>
+      <c r="G193">
+        <v>1</v>
+      </c>
+      <c r="H193" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L193" s="1">
+        <v>3</v>
+      </c>
+      <c r="R193">
+        <v>1</v>
+      </c>
+      <c r="S193" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="194" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A194" s="1">
+        <v>4</v>
+      </c>
+      <c r="G194">
+        <v>1</v>
+      </c>
+      <c r="H194" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L194" s="1">
+        <v>4</v>
+      </c>
+      <c r="R194">
+        <v>1</v>
+      </c>
+      <c r="S194" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="195" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A195" s="1">
+        <v>5</v>
+      </c>
+      <c r="G195">
+        <v>1</v>
+      </c>
+      <c r="H195" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L195" s="1">
+        <v>5</v>
+      </c>
+      <c r="R195">
+        <v>1</v>
+      </c>
+      <c r="S195" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="196" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A196" s="1">
+        <v>6</v>
+      </c>
+      <c r="G196">
+        <v>1</v>
+      </c>
+      <c r="H196" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L196" s="1">
+        <v>6</v>
+      </c>
+      <c r="R196">
+        <v>1</v>
+      </c>
+      <c r="S196" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="197" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A197" s="1">
+        <v>7</v>
+      </c>
+      <c r="G197">
+        <v>1</v>
+      </c>
+      <c r="H197" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L197" s="1">
+        <v>7</v>
+      </c>
+      <c r="R197">
+        <v>1</v>
+      </c>
+      <c r="S197" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="198" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A198" s="1">
+        <v>8</v>
+      </c>
+      <c r="G198">
+        <v>1</v>
+      </c>
+      <c r="H198" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L198" s="1">
+        <v>8</v>
+      </c>
+      <c r="R198">
+        <v>1</v>
+      </c>
+      <c r="S198" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="199" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A199" s="4">
+        <v>9</v>
+      </c>
+      <c r="G199">
+        <v>1</v>
+      </c>
+      <c r="H199" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L199" s="4">
+        <v>9</v>
+      </c>
+      <c r="R199">
+        <v>1</v>
+      </c>
+      <c r="S199" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="200" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A200" s="1">
+        <v>10</v>
+      </c>
+      <c r="G200">
+        <v>1</v>
+      </c>
+      <c r="H200" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L200" s="1">
+        <v>10</v>
+      </c>
+      <c r="R200">
+        <v>1</v>
+      </c>
+      <c r="S200" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="201" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A201" s="1">
+        <v>11</v>
+      </c>
+      <c r="B201" s="16"/>
+      <c r="D201" s="16"/>
+      <c r="G201">
+        <v>0.05</v>
+      </c>
+      <c r="H201" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L201" s="1">
+        <v>11</v>
+      </c>
+      <c r="R201">
+        <v>0.05</v>
+      </c>
+      <c r="S201" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="202" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A202" s="1">
+        <v>12</v>
+      </c>
+      <c r="G202">
+        <v>0.05</v>
+      </c>
+      <c r="H202" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L202" s="1">
+        <v>12</v>
+      </c>
+      <c r="R202">
+        <v>0.05</v>
+      </c>
+      <c r="S202" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="203" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A203" s="1">
+        <v>13</v>
+      </c>
+      <c r="G203">
+        <v>0.05</v>
+      </c>
+      <c r="H203" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L203" s="1">
+        <v>13</v>
+      </c>
+      <c r="R203">
+        <v>0.05</v>
+      </c>
+      <c r="S203" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="204" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A204" s="1">
+        <v>14</v>
+      </c>
+      <c r="G204">
+        <v>0.05</v>
+      </c>
+      <c r="H204" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L204" s="1">
+        <v>14</v>
+      </c>
+      <c r="R204">
+        <v>0.05</v>
+      </c>
+      <c r="S204" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="205" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A205" s="1">
+        <v>15</v>
+      </c>
+      <c r="G205">
+        <v>0.05</v>
+      </c>
+      <c r="H205" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L205" s="1">
+        <v>15</v>
+      </c>
+      <c r="R205">
+        <v>0.05</v>
+      </c>
+      <c r="S205" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="206" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A206" s="1">
+        <v>16</v>
+      </c>
+      <c r="G206">
+        <v>0.05</v>
+      </c>
+      <c r="H206" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L206" s="1">
+        <v>16</v>
+      </c>
+      <c r="R206">
+        <v>0.05</v>
+      </c>
+      <c r="S206" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="207" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A207" s="1">
+        <v>17</v>
+      </c>
+      <c r="G207">
+        <v>0.05</v>
+      </c>
+      <c r="H207" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L207" s="1">
+        <v>17</v>
+      </c>
+      <c r="R207">
+        <v>0.05</v>
+      </c>
+      <c r="S207" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="208" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A208" s="1">
+        <v>18</v>
+      </c>
+      <c r="G208">
+        <v>0.05</v>
+      </c>
+      <c r="H208" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L208" s="1">
+        <v>18</v>
+      </c>
+      <c r="R208">
+        <v>0.05</v>
+      </c>
+      <c r="S208" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="209" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A209" s="1">
+        <v>19</v>
+      </c>
+      <c r="G209">
+        <v>0.05</v>
+      </c>
+      <c r="H209" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L209" s="1">
+        <v>19</v>
+      </c>
+      <c r="R209">
+        <v>0.05</v>
+      </c>
+      <c r="S209" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="210" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A210" s="1">
+        <v>20</v>
+      </c>
+      <c r="G210">
+        <v>0.05</v>
+      </c>
+      <c r="H210" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L210" s="1">
+        <v>20</v>
+      </c>
+      <c r="R210">
+        <v>0.05</v>
+      </c>
+      <c r="S210" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="211" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A211" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B211" s="7"/>
+    </row>
+    <row r="212" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A212" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="L212" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="213" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="L213" s="6" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sink speed results are added (RL)
</commit_message>
<xml_diff>
--- a/pyFiles/RL/Results/New Results/ResultsDQNfixEpsilon.xlsx
+++ b/pyFiles/RL/Results/New Results/ResultsDQNfixEpsilon.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bozho1\Desktop\Thesis Code\ThesisWorkCybercom\pyFiles\RL\Results\New Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{729A3D91-2F0E-48EF-9BBC-3C4B1985314F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC73190F-F000-49E8-B2D2-500BD9CCBB59}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1BC5E51A-5632-4252-887C-9C128D35FB87}"/>
   </bookViews>
@@ -594,10 +594,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2693EA75-5C63-4FDE-887F-C7326CFE699C}">
-  <dimension ref="A1:AN213"/>
+  <dimension ref="A1:AN212"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A128" workbookViewId="0">
-      <selection activeCell="H216" sqref="H216"/>
+    <sheetView tabSelected="1" topLeftCell="A167" workbookViewId="0">
+      <selection activeCell="E186" sqref="E186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10569,6 +10569,19 @@
       <c r="A176" s="1">
         <v>11</v>
       </c>
+      <c r="B176">
+        <v>4080</v>
+      </c>
+      <c r="C176" s="16">
+        <v>22</v>
+      </c>
+      <c r="D176">
+        <v>1.6245023999999899</v>
+      </c>
+      <c r="E176">
+        <f>B176/D176</f>
+        <v>2511.5383024365033</v>
+      </c>
       <c r="G176">
         <v>0.05</v>
       </c>
@@ -10577,6 +10590,19 @@
       </c>
       <c r="L176" s="1">
         <v>11</v>
+      </c>
+      <c r="M176">
+        <v>15293</v>
+      </c>
+      <c r="N176">
+        <v>170</v>
+      </c>
+      <c r="O176">
+        <v>4.9999999999999902</v>
+      </c>
+      <c r="P176">
+        <f>M176/O176</f>
+        <v>3058.6000000000058</v>
       </c>
       <c r="R176">
         <v>0.05</v>
@@ -10589,6 +10615,19 @@
       <c r="A177" s="1">
         <v>12</v>
       </c>
+      <c r="B177">
+        <v>5116</v>
+      </c>
+      <c r="C177">
+        <v>27</v>
+      </c>
+      <c r="D177">
+        <v>2.1356321</v>
+      </c>
+      <c r="E177">
+        <f t="shared" ref="E177:E187" si="18">B177/D177</f>
+        <v>2395.5436893835786</v>
+      </c>
       <c r="G177">
         <v>0.05</v>
       </c>
@@ -10597,6 +10636,19 @@
       </c>
       <c r="L177" s="1">
         <v>12</v>
+      </c>
+      <c r="M177">
+        <v>16241</v>
+      </c>
+      <c r="N177">
+        <v>334</v>
+      </c>
+      <c r="O177">
+        <v>4.9999999999999902</v>
+      </c>
+      <c r="P177">
+        <f t="shared" ref="P177:P187" si="19">M177/O177</f>
+        <v>3248.2000000000062</v>
       </c>
       <c r="R177">
         <v>0.05</v>
@@ -10609,6 +10661,19 @@
       <c r="A178" s="1">
         <v>13</v>
       </c>
+      <c r="B178">
+        <v>3169</v>
+      </c>
+      <c r="C178">
+        <v>17</v>
+      </c>
+      <c r="D178">
+        <v>1.48072099999999</v>
+      </c>
+      <c r="E178">
+        <f t="shared" si="18"/>
+        <v>2140.1736046156038</v>
+      </c>
       <c r="G178">
         <v>0.05</v>
       </c>
@@ -10617,6 +10682,19 @@
       </c>
       <c r="L178" s="1">
         <v>13</v>
+      </c>
+      <c r="M178">
+        <v>14255</v>
+      </c>
+      <c r="N178">
+        <v>324</v>
+      </c>
+      <c r="O178">
+        <v>4.9999999999999902</v>
+      </c>
+      <c r="P178">
+        <f t="shared" si="19"/>
+        <v>2851.0000000000055</v>
       </c>
       <c r="R178">
         <v>0.05</v>
@@ -10629,6 +10707,19 @@
       <c r="A179" s="1">
         <v>14</v>
       </c>
+      <c r="B179">
+        <v>6893</v>
+      </c>
+      <c r="C179">
+        <v>37</v>
+      </c>
+      <c r="D179">
+        <v>2.57983329999999</v>
+      </c>
+      <c r="E179">
+        <f t="shared" si="18"/>
+        <v>2671.8780628190307</v>
+      </c>
       <c r="G179">
         <v>0.05</v>
       </c>
@@ -10637,6 +10728,19 @@
       </c>
       <c r="L179" s="1">
         <v>14</v>
+      </c>
+      <c r="M179">
+        <v>12571</v>
+      </c>
+      <c r="N179">
+        <v>165</v>
+      </c>
+      <c r="O179">
+        <v>4.9999999999999902</v>
+      </c>
+      <c r="P179">
+        <f t="shared" si="19"/>
+        <v>2514.2000000000048</v>
       </c>
       <c r="R179">
         <v>0.05</v>
@@ -10649,6 +10753,19 @@
       <c r="A180" s="1">
         <v>15</v>
       </c>
+      <c r="B180">
+        <v>5616</v>
+      </c>
+      <c r="C180">
+        <v>30</v>
+      </c>
+      <c r="D180">
+        <v>2.1950238999999998</v>
+      </c>
+      <c r="E180">
+        <f t="shared" si="18"/>
+        <v>2558.5142831474413</v>
+      </c>
       <c r="G180">
         <v>0.05</v>
       </c>
@@ -10657,6 +10774,19 @@
       </c>
       <c r="L180" s="1">
         <v>15</v>
+      </c>
+      <c r="M180">
+        <v>18758</v>
+      </c>
+      <c r="N180">
+        <v>354</v>
+      </c>
+      <c r="O180">
+        <v>4.9999999999999902</v>
+      </c>
+      <c r="P180">
+        <f t="shared" si="19"/>
+        <v>3751.6000000000072</v>
       </c>
       <c r="R180">
         <v>0.05</v>
@@ -10669,6 +10799,19 @@
       <c r="A181" s="1">
         <v>16</v>
       </c>
+      <c r="B181">
+        <v>5055</v>
+      </c>
+      <c r="C181">
+        <v>27</v>
+      </c>
+      <c r="D181">
+        <v>2.1003627999999899</v>
+      </c>
+      <c r="E181">
+        <f t="shared" si="18"/>
+        <v>2406.727066390637</v>
+      </c>
       <c r="G181">
         <v>0.05</v>
       </c>
@@ -10677,6 +10820,19 @@
       </c>
       <c r="L181" s="1">
         <v>16</v>
+      </c>
+      <c r="M181">
+        <v>15679</v>
+      </c>
+      <c r="N181">
+        <v>331</v>
+      </c>
+      <c r="O181">
+        <v>4.9999999999999902</v>
+      </c>
+      <c r="P181">
+        <f t="shared" si="19"/>
+        <v>3135.8000000000061</v>
       </c>
       <c r="R181">
         <v>0.05</v>
@@ -10689,6 +10845,19 @@
       <c r="A182" s="1">
         <v>17</v>
       </c>
+      <c r="B182">
+        <v>4802</v>
+      </c>
+      <c r="C182">
+        <v>26</v>
+      </c>
+      <c r="D182">
+        <v>2.09389289999999</v>
+      </c>
+      <c r="E182">
+        <f t="shared" si="18"/>
+        <v>2293.3360154189468</v>
+      </c>
       <c r="G182">
         <v>0.05</v>
       </c>
@@ -10697,6 +10866,19 @@
       </c>
       <c r="L182" s="1">
         <v>17</v>
+      </c>
+      <c r="M182">
+        <v>13771</v>
+      </c>
+      <c r="N182">
+        <v>211</v>
+      </c>
+      <c r="O182">
+        <v>4.9999999999999902</v>
+      </c>
+      <c r="P182">
+        <f t="shared" si="19"/>
+        <v>2754.2000000000053</v>
       </c>
       <c r="R182">
         <v>0.05</v>
@@ -10709,6 +10891,19 @@
       <c r="A183" s="1">
         <v>18</v>
       </c>
+      <c r="B183">
+        <v>4381</v>
+      </c>
+      <c r="C183">
+        <v>23</v>
+      </c>
+      <c r="D183">
+        <v>1.70647119999999</v>
+      </c>
+      <c r="E183">
+        <f t="shared" si="18"/>
+        <v>2567.2862220001284</v>
+      </c>
       <c r="G183">
         <v>0.05</v>
       </c>
@@ -10717,6 +10912,19 @@
       </c>
       <c r="L183" s="1">
         <v>18</v>
+      </c>
+      <c r="M183">
+        <v>14884</v>
+      </c>
+      <c r="N183">
+        <v>145</v>
+      </c>
+      <c r="O183">
+        <v>4.9999999999999902</v>
+      </c>
+      <c r="P183">
+        <f t="shared" si="19"/>
+        <v>2976.8000000000056</v>
       </c>
       <c r="R183">
         <v>0.05</v>
@@ -10729,6 +10937,19 @@
       <c r="A184" s="1">
         <v>19</v>
       </c>
+      <c r="B184">
+        <v>3956</v>
+      </c>
+      <c r="C184">
+        <v>21</v>
+      </c>
+      <c r="D184">
+        <v>1.6813514999999899</v>
+      </c>
+      <c r="E184">
+        <f t="shared" si="18"/>
+        <v>2352.869105597505</v>
+      </c>
       <c r="G184">
         <v>0.05</v>
       </c>
@@ -10737,6 +10958,19 @@
       </c>
       <c r="L184" s="1">
         <v>19</v>
+      </c>
+      <c r="M184">
+        <v>17929</v>
+      </c>
+      <c r="N184">
+        <v>170</v>
+      </c>
+      <c r="O184">
+        <v>4.9999999999999902</v>
+      </c>
+      <c r="P184">
+        <f t="shared" si="19"/>
+        <v>3585.800000000007</v>
       </c>
       <c r="R184">
         <v>0.05</v>
@@ -10749,6 +10983,19 @@
       <c r="A185" s="1">
         <v>20</v>
       </c>
+      <c r="B185">
+        <v>4289</v>
+      </c>
+      <c r="C185">
+        <v>23</v>
+      </c>
+      <c r="D185">
+        <v>1.9395910999999899</v>
+      </c>
+      <c r="E185">
+        <f t="shared" si="18"/>
+        <v>2211.29082310185</v>
+      </c>
       <c r="G185">
         <v>0.05</v>
       </c>
@@ -10757,6 +11004,19 @@
       </c>
       <c r="L185" s="1">
         <v>20</v>
+      </c>
+      <c r="M185">
+        <v>16655</v>
+      </c>
+      <c r="N185">
+        <v>173</v>
+      </c>
+      <c r="O185">
+        <v>4.9999999999999902</v>
+      </c>
+      <c r="P185">
+        <f t="shared" si="19"/>
+        <v>3331.0000000000064</v>
       </c>
       <c r="R185">
         <v>0.05</v>
@@ -10777,12 +11037,39 @@
       <c r="A187" s="6" t="s">
         <v>16</v>
       </c>
+      <c r="B187">
+        <v>4735.7</v>
+      </c>
+      <c r="C187">
+        <v>25.3</v>
+      </c>
+      <c r="D187">
+        <v>1.95373821999999</v>
+      </c>
+      <c r="E187">
+        <f t="shared" si="18"/>
+        <v>2423.9173659611492</v>
+      </c>
       <c r="L187" s="6" t="s">
         <v>16</v>
       </c>
+      <c r="M187">
+        <v>15603.6</v>
+      </c>
+      <c r="N187">
+        <v>237.7</v>
+      </c>
+      <c r="O187">
+        <v>4.9999999999999902</v>
+      </c>
+      <c r="P187">
+        <f t="shared" si="19"/>
+        <v>3120.7200000000062</v>
+      </c>
     </row>
     <row r="188" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B188" s="6"/>
+      <c r="C188" s="7"/>
     </row>
     <row r="190" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A190" s="6" t="s">
@@ -10996,8 +11283,19 @@
       <c r="A201" s="1">
         <v>11</v>
       </c>
-      <c r="B201" s="16"/>
-      <c r="D201" s="16"/>
+      <c r="B201">
+        <v>4024</v>
+      </c>
+      <c r="C201">
+        <v>22</v>
+      </c>
+      <c r="D201">
+        <v>0.73214820000000003</v>
+      </c>
+      <c r="E201">
+        <f>B201/D201</f>
+        <v>5496.1550134248773</v>
+      </c>
       <c r="G201">
         <v>0.05</v>
       </c>
@@ -11006,6 +11304,19 @@
       </c>
       <c r="L201" s="1">
         <v>11</v>
+      </c>
+      <c r="M201">
+        <v>32964</v>
+      </c>
+      <c r="N201">
+        <v>428</v>
+      </c>
+      <c r="O201">
+        <v>4.9999999999999902</v>
+      </c>
+      <c r="P201">
+        <f>M201/O201</f>
+        <v>6592.8000000000129</v>
       </c>
       <c r="R201">
         <v>0.05</v>
@@ -11018,6 +11329,19 @@
       <c r="A202" s="1">
         <v>12</v>
       </c>
+      <c r="B202">
+        <v>5019</v>
+      </c>
+      <c r="C202">
+        <v>27</v>
+      </c>
+      <c r="D202">
+        <v>0.89836909999999903</v>
+      </c>
+      <c r="E202">
+        <f t="shared" ref="E202:E212" si="20">B202/D202</f>
+        <v>5586.7905519012238</v>
+      </c>
       <c r="G202">
         <v>0.05</v>
       </c>
@@ -11026,6 +11350,19 @@
       </c>
       <c r="L202" s="1">
         <v>12</v>
+      </c>
+      <c r="M202">
+        <v>33970</v>
+      </c>
+      <c r="N202">
+        <v>403</v>
+      </c>
+      <c r="O202">
+        <v>4.9999999999999902</v>
+      </c>
+      <c r="P202">
+        <f t="shared" ref="P202:P213" si="21">M202/O202</f>
+        <v>6794.0000000000136</v>
       </c>
       <c r="R202">
         <v>0.05</v>
@@ -11038,6 +11375,19 @@
       <c r="A203" s="1">
         <v>13</v>
       </c>
+      <c r="B203">
+        <v>3114</v>
+      </c>
+      <c r="C203">
+        <v>17</v>
+      </c>
+      <c r="D203">
+        <v>0.56991760000000002</v>
+      </c>
+      <c r="E203">
+        <f t="shared" si="20"/>
+        <v>5463.9477706952721</v>
+      </c>
       <c r="G203">
         <v>0.05</v>
       </c>
@@ -11046,6 +11396,19 @@
       </c>
       <c r="L203" s="1">
         <v>13</v>
+      </c>
+      <c r="M203">
+        <v>32846</v>
+      </c>
+      <c r="N203">
+        <v>417</v>
+      </c>
+      <c r="O203">
+        <v>4.9999999999999902</v>
+      </c>
+      <c r="P203">
+        <f t="shared" si="21"/>
+        <v>6569.2000000000126</v>
       </c>
       <c r="R203">
         <v>0.05</v>
@@ -11058,6 +11421,19 @@
       <c r="A204" s="1">
         <v>14</v>
       </c>
+      <c r="B204">
+        <v>6893</v>
+      </c>
+      <c r="C204">
+        <v>37</v>
+      </c>
+      <c r="D204">
+        <v>1.2542549000000001</v>
+      </c>
+      <c r="E204">
+        <f t="shared" si="20"/>
+        <v>5495.693100341884</v>
+      </c>
       <c r="G204">
         <v>0.05</v>
       </c>
@@ -11066,6 +11442,19 @@
       </c>
       <c r="L204" s="1">
         <v>14</v>
+      </c>
+      <c r="M204">
+        <v>33205</v>
+      </c>
+      <c r="N204">
+        <v>425</v>
+      </c>
+      <c r="O204">
+        <v>4.9999999999999902</v>
+      </c>
+      <c r="P204">
+        <f t="shared" si="21"/>
+        <v>6641.0000000000127</v>
       </c>
       <c r="R204">
         <v>0.05</v>
@@ -11078,6 +11467,19 @@
       <c r="A205" s="1">
         <v>15</v>
       </c>
+      <c r="B205">
+        <v>5613</v>
+      </c>
+      <c r="C205">
+        <v>30</v>
+      </c>
+      <c r="D205">
+        <v>0.93838729999999904</v>
+      </c>
+      <c r="E205">
+        <f t="shared" si="20"/>
+        <v>5981.5387527090425</v>
+      </c>
       <c r="G205">
         <v>0.05</v>
       </c>
@@ -11086,6 +11488,19 @@
       </c>
       <c r="L205" s="1">
         <v>15</v>
+      </c>
+      <c r="M205">
+        <v>31588</v>
+      </c>
+      <c r="N205">
+        <v>386</v>
+      </c>
+      <c r="O205">
+        <v>4.9999999999999902</v>
+      </c>
+      <c r="P205">
+        <f t="shared" si="21"/>
+        <v>6317.6000000000122</v>
       </c>
       <c r="R205">
         <v>0.05</v>
@@ -11098,6 +11513,19 @@
       <c r="A206" s="1">
         <v>16</v>
       </c>
+      <c r="B206">
+        <v>5057</v>
+      </c>
+      <c r="C206">
+        <v>27</v>
+      </c>
+      <c r="D206">
+        <v>0.90773760000000003</v>
+      </c>
+      <c r="E206">
+        <f t="shared" si="20"/>
+        <v>5570.993203322193</v>
+      </c>
       <c r="G206">
         <v>0.05</v>
       </c>
@@ -11106,6 +11534,19 @@
       </c>
       <c r="L206" s="1">
         <v>16</v>
+      </c>
+      <c r="M206">
+        <v>31216</v>
+      </c>
+      <c r="N206">
+        <v>436</v>
+      </c>
+      <c r="O206">
+        <v>4.9999999999999902</v>
+      </c>
+      <c r="P206">
+        <f t="shared" si="21"/>
+        <v>6243.2000000000126</v>
       </c>
       <c r="R206">
         <v>0.05</v>
@@ -11118,6 +11559,19 @@
       <c r="A207" s="1">
         <v>17</v>
       </c>
+      <c r="B207">
+        <v>4780</v>
+      </c>
+      <c r="C207">
+        <v>26</v>
+      </c>
+      <c r="D207">
+        <v>0.82166700000000004</v>
+      </c>
+      <c r="E207">
+        <f t="shared" si="20"/>
+        <v>5817.4418590499554</v>
+      </c>
       <c r="G207">
         <v>0.05</v>
       </c>
@@ -11126,6 +11580,19 @@
       </c>
       <c r="L207" s="1">
         <v>17</v>
+      </c>
+      <c r="M207">
+        <v>34591</v>
+      </c>
+      <c r="N207">
+        <v>405</v>
+      </c>
+      <c r="O207">
+        <v>4.9999999999999902</v>
+      </c>
+      <c r="P207">
+        <f t="shared" si="21"/>
+        <v>6918.2000000000135</v>
       </c>
       <c r="R207">
         <v>0.05</v>
@@ -11138,6 +11605,19 @@
       <c r="A208" s="1">
         <v>18</v>
       </c>
+      <c r="B208">
+        <v>4309</v>
+      </c>
+      <c r="C208">
+        <v>23</v>
+      </c>
+      <c r="D208">
+        <v>0.7910992</v>
+      </c>
+      <c r="E208">
+        <f t="shared" si="20"/>
+        <v>5446.8516716993263</v>
+      </c>
       <c r="G208">
         <v>0.05</v>
       </c>
@@ -11146,6 +11626,19 @@
       </c>
       <c r="L208" s="1">
         <v>18</v>
+      </c>
+      <c r="M208">
+        <v>32594</v>
+      </c>
+      <c r="N208">
+        <v>430</v>
+      </c>
+      <c r="O208">
+        <v>4.9999999999999902</v>
+      </c>
+      <c r="P208">
+        <f t="shared" si="21"/>
+        <v>6518.8000000000129</v>
       </c>
       <c r="R208">
         <v>0.05</v>
@@ -11158,6 +11651,19 @@
       <c r="A209" s="1">
         <v>19</v>
       </c>
+      <c r="B209">
+        <v>3916</v>
+      </c>
+      <c r="C209">
+        <v>21</v>
+      </c>
+      <c r="D209">
+        <v>0.74726840000000005</v>
+      </c>
+      <c r="E209">
+        <f t="shared" si="20"/>
+        <v>5240.4196403862379</v>
+      </c>
       <c r="G209">
         <v>0.05</v>
       </c>
@@ -11166,6 +11672,19 @@
       </c>
       <c r="L209" s="1">
         <v>19</v>
+      </c>
+      <c r="M209">
+        <v>31033</v>
+      </c>
+      <c r="N209">
+        <v>439</v>
+      </c>
+      <c r="O209">
+        <v>4.9999999999999902</v>
+      </c>
+      <c r="P209">
+        <f t="shared" si="21"/>
+        <v>6206.6000000000122</v>
       </c>
       <c r="R209">
         <v>0.05</v>
@@ -11178,6 +11697,19 @@
       <c r="A210" s="1">
         <v>20</v>
       </c>
+      <c r="B210">
+        <v>4228</v>
+      </c>
+      <c r="C210">
+        <v>23</v>
+      </c>
+      <c r="D210">
+        <v>0.78835560000000005</v>
+      </c>
+      <c r="E210">
+        <f t="shared" si="20"/>
+        <v>5363.0620496638821</v>
+      </c>
       <c r="G210">
         <v>0.05</v>
       </c>
@@ -11186,6 +11718,19 @@
       </c>
       <c r="L210" s="1">
         <v>20</v>
+      </c>
+      <c r="M210">
+        <v>31338</v>
+      </c>
+      <c r="N210">
+        <v>439</v>
+      </c>
+      <c r="O210">
+        <v>4.9999999999999902</v>
+      </c>
+      <c r="P210">
+        <f t="shared" si="21"/>
+        <v>6267.6000000000122</v>
       </c>
       <c r="R210">
         <v>0.05</v>
@@ -11199,18 +11744,42 @@
         <v>15</v>
       </c>
       <c r="B211" s="7"/>
+      <c r="L211" s="6" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="212" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A212" s="6" t="s">
         <v>16</v>
       </c>
+      <c r="B212">
+        <v>4695.3</v>
+      </c>
+      <c r="C212">
+        <v>25.3</v>
+      </c>
+      <c r="D212">
+        <v>0.84492049000000002</v>
+      </c>
+      <c r="E212">
+        <f t="shared" si="20"/>
+        <v>5557.0909400007567</v>
+      </c>
       <c r="L212" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="213" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="L213" s="6" t="s">
         <v>16</v>
+      </c>
+      <c r="M212">
+        <v>32534.5</v>
+      </c>
+      <c r="N212">
+        <v>420.8</v>
+      </c>
+      <c r="O212">
+        <v>4.9999999999999902</v>
+      </c>
+      <c r="P212">
+        <f>M212/O212</f>
+        <v>6506.9000000000124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>